<commit_message>
Selected another equivalent parts to cover shortage
</commit_message>
<xml_diff>
--- a/cam/RP2040-Eins-20231112-JLCPCB-BOM-SOIC.xlsx
+++ b/cam/RP2040-Eins-20231112-JLCPCB-BOM-SOIC.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26827"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26924"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\AG\Documents\KiCad\7.0\projects\RP2040-Eins\cam\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{138A143D-BAB0-48E9-9E77-03586DE220BC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E4BBE456-5748-49AF-83C7-9C0A236AC60A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="11040" yWindow="3636" windowWidth="12336" windowHeight="18756" xr2:uid="{7B845E16-6401-438E-89AD-84A195B2B6BE}"/>
+    <workbookView xWindow="372" yWindow="1644" windowWidth="12336" windowHeight="18756" xr2:uid="{7B845E16-6401-438E-89AD-84A195B2B6BE}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -334,9 +334,6 @@
     <t>C15127</t>
   </si>
   <si>
-    <t>C377102</t>
-  </si>
-  <si>
     <t>C5158049</t>
   </si>
   <si>
@@ -388,10 +385,13 @@
     <t>C40877</t>
   </si>
   <si>
-    <t>C920875</t>
-  </si>
-  <si>
     <t>C2685154</t>
+  </si>
+  <si>
+    <t>C2935953</t>
+  </si>
+  <si>
+    <t>C106074</t>
   </si>
 </sst>
 </file>
@@ -758,7 +758,7 @@
   <dimension ref="A1:E32"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D32" sqref="D32"/>
+      <selection activeCell="D29" sqref="D29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -894,16 +894,16 @@
         <v>1</v>
       </c>
       <c r="B8" t="s">
+        <v>99</v>
+      </c>
+      <c r="C8" s="2" t="s">
+        <v>101</v>
+      </c>
+      <c r="D8" t="s">
+        <v>98</v>
+      </c>
+      <c r="E8" t="s">
         <v>100</v>
-      </c>
-      <c r="C8" s="2" t="s">
-        <v>102</v>
-      </c>
-      <c r="D8" t="s">
-        <v>99</v>
-      </c>
-      <c r="E8" t="s">
-        <v>101</v>
       </c>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.3">
@@ -914,10 +914,10 @@
         <v>14</v>
       </c>
       <c r="C9" s="2" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="D9" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="E9" t="s">
         <v>15</v>
@@ -931,10 +931,10 @@
         <v>16</v>
       </c>
       <c r="C10" s="2" t="s">
+        <v>103</v>
+      </c>
+      <c r="D10" t="s">
         <v>104</v>
-      </c>
-      <c r="D10" t="s">
-        <v>105</v>
       </c>
       <c r="E10" t="s">
         <v>17</v>
@@ -988,7 +988,7 @@
         <v>84</v>
       </c>
       <c r="E13" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.3">
@@ -1070,7 +1070,7 @@
         <v>65</v>
       </c>
       <c r="D18" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="E18" t="s">
         <v>32</v>
@@ -1101,10 +1101,10 @@
         <v>35</v>
       </c>
       <c r="C20" s="2" t="s">
+        <v>105</v>
+      </c>
+      <c r="D20" t="s">
         <v>106</v>
-      </c>
-      <c r="D20" t="s">
-        <v>107</v>
       </c>
       <c r="E20" t="s">
         <v>36</v>
@@ -1115,7 +1115,7 @@
         <v>4</v>
       </c>
       <c r="B21" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="C21" s="2" t="s">
         <v>81</v>
@@ -1135,10 +1135,10 @@
         <v>38</v>
       </c>
       <c r="C22" s="2" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="D22" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="E22" t="s">
         <v>39</v>
@@ -1152,10 +1152,10 @@
         <v>40</v>
       </c>
       <c r="C23" s="2" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="D23" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="E23" t="s">
         <v>41</v>
@@ -1203,10 +1203,10 @@
         <v>45</v>
       </c>
       <c r="C26" s="2" t="s">
+        <v>101</v>
+      </c>
+      <c r="D26" t="s">
         <v>102</v>
-      </c>
-      <c r="D26" t="s">
-        <v>103</v>
       </c>
       <c r="E26" t="s">
         <v>46</v>
@@ -1240,7 +1240,7 @@
         <v>66</v>
       </c>
       <c r="D28" t="s">
-        <v>95</v>
+        <v>114</v>
       </c>
       <c r="E28" t="s">
         <v>50</v>
@@ -1257,7 +1257,7 @@
         <v>52</v>
       </c>
       <c r="D29" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="E29" t="s">
         <v>53</v>
@@ -1271,10 +1271,10 @@
         <v>54</v>
       </c>
       <c r="C30" s="2" t="s">
+        <v>105</v>
+      </c>
+      <c r="D30" t="s">
         <v>106</v>
-      </c>
-      <c r="D30" t="s">
-        <v>107</v>
       </c>
       <c r="E30" t="s">
         <v>55</v>
@@ -1291,7 +1291,7 @@
         <v>64</v>
       </c>
       <c r="D31" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="E31" t="s">
         <v>57</v>
@@ -1305,10 +1305,10 @@
         <v>58</v>
       </c>
       <c r="C32" s="2" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="D32" t="s">
-        <v>114</v>
+        <v>112</v>
       </c>
       <c r="E32" t="s">
         <v>59</v>

</xml_diff>